<commit_message>
Updated locations based on sampling around site
</commit_message>
<xml_diff>
--- a/Hall_A-GEn-E12-09-016.xlsx
+++ b/Hall_A-GEn-E12-09-016.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,36 +449,6 @@
           <t>dose_rate-1</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>dose_rate-2</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>dose_rate-3</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>dose_rate-4</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>dose_rate-5</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>dose_rate-6</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>dose_rate-7</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -486,32 +456,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RBM 1</t>
+          <t>RBM 3</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>247.53</v>
+        <v>179.2</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3370879700075959</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1.486771269912188</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.2540038137441724</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.0377426827622672</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.3370879700075959</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.3880001987170133</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.4269751776618813</v>
+        <v>0.1606729401023607</v>
       </c>
     </row>
     <row r="3">
@@ -527,25 +479,7 @@
         <v>199.03</v>
       </c>
       <c r="D3" t="n">
-        <v>0.525454602642478</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2.317587325452039</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.3959425577175316</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.05883350382709095</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.525454602642478</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.6045080880589819</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.6652314848046758</v>
+        <v>0.1310690645894549</v>
       </c>
     </row>
     <row r="4">
@@ -554,32 +488,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RBM 3</t>
+          <t>RBM 1</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>179.2</v>
+        <v>247.53</v>
       </c>
       <c r="D4" t="n">
-        <v>0.644136251077488</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2.841048501343351</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.485372006425708</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.07212191577037259</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.644136251077488</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.7408904193471172</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.815313547453732</v>
+        <v>0.08408301057991752</v>
       </c>
     </row>
     <row r="5">
@@ -595,25 +511,7 @@
         <v>398.027</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1152883599879308</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.5084946264367932</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.08687252504616408</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.01290847607853962</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.1152883599879308</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.1329114336315477</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.1462625101115368</v>
+        <v>0.02875745578339117</v>
       </c>
     </row>
     <row r="6">
@@ -629,25 +527,7 @@
         <v>836.75</v>
       </c>
       <c r="D6" t="n">
-        <v>0.01467505837204829</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.06472629435976035</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.01105800599568895</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.001643120259205604</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.01467505837204829</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.01699663289547831</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.01870396039537496</v>
+        <v>0.003660537302265751</v>
       </c>
     </row>
     <row r="7">
@@ -663,25 +543,503 @@
         <v>672.58</v>
       </c>
       <c r="D7" t="n">
-        <v>0.02858255220674847</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.1260671433655768</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.02153763383158534</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.00320029872454641</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.02858255220674847</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.03304709980692758</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.03636671155821784</v>
+        <v>0.007129613790569032</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>87.15649859</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.5499251280565078</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>256.7333627</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.07784071189344753</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>208.8065396</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1191692841813518</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>252.2829526</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.08077914618229871</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>137.4515881</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.2613929346285209</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>136.9984942</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.2629156981209262</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>44.07944661</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.343743765675084</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>229.3342048</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.09854191647972506</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>254.9305337</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.07901360202502992</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>162.8349264</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.1924187707764591</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>239.5514598</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.09004707370218711</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>105.264492</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.4098178123184146</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>156.7215217</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.2064925568359615</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>130.3022313</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.2869318514442246</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>142.1112766</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.2464187593464372</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>296.5991319</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.05690347256499718</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>210.1468805</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.117653337004932</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>123.0649137</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.3164629220484221</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>217.6836627</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.1095964761209652</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>158.3857689</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.2025245720457831</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>171.2175902</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.175180113782256</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>207.1589799</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.1210691238693947</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>238.6422275</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.09076227370710256</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>63.67301683</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.8576369169547265</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>234.1731468</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.09439055090088236</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>rad48_p1</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>33.91246784</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1.766192861138571</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>rad43_p1</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>117.6931463</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.3411922084878132</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>rad46_p1</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>150.1850724</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.2231580422614551</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>rad47_p1</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>102.3597591</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.4286191754995735</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>rad41_p1</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>198.2259958</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.1321182084034843</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>rad34_p1</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>72.30364910999999</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.7212635140073126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>